<commit_message>
Agregados casos de prueba faltantes a planilla
</commit_message>
<xml_diff>
--- a/Documentación/Casos de Prueba.xlsx
+++ b/Documentación/Casos de Prueba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCTACHU\workspace\DDS2016\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ariel\Documents\GitHub\DDS2016\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="79">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -39,192 +39,108 @@
     <t>Consultar por cercanía</t>
   </si>
   <si>
-    <t>La geolocalización no pertenece a la comuna del CGP</t>
-  </si>
-  <si>
     <t>El POI no debe ser cercano</t>
   </si>
   <si>
     <t>OK</t>
   </si>
   <si>
-    <t>CGP - dadaUnaGeolocalizacionDentroDelRangoEsCercanoDebeDevolverTrue</t>
-  </si>
-  <si>
     <t>La Geolocalización pertenece a la comuna del CGP</t>
   </si>
   <si>
     <t>El POI debe ser cercano</t>
   </si>
   <si>
-    <t>LocalComercial - dadaUnaGeolocalizacionFueraDelRangoLibreriaEscolarNoDebeSerCercana</t>
-  </si>
-  <si>
     <t>La Geolocalización supera el radio de cercanía del rubro del local comercial</t>
   </si>
   <si>
-    <t>LocalComercial - dadaUnaGeolocalizacionDentroDelRangoLibreriaEscolarDebeSerCercana</t>
-  </si>
-  <si>
     <t>La Geolocalización no supera el radio de cercanía del rubro del local comercial</t>
   </si>
   <si>
-    <t>ParadaColectivo - dadaUnaGeolocalizacionFueraDelRangoEsCercanoDebeDevolverFalse</t>
-  </si>
-  <si>
     <t>La Geolocalización se encuentra a más de 1 cuadra de la parada de colectivo</t>
   </si>
   <si>
-    <t>ParadaColectivo - dadaUnaGeolocalizacionDentroDelRangoEsCercanoDebeDevolverTrue</t>
-  </si>
-  <si>
     <t>La Geolocalización se encuentra a menos de 1 cuadra de la parada de colectivo</t>
   </si>
   <si>
-    <t>SucursalBanco - dadaUnaGeolocalizacionFueraDelRangoEsCercanoDebeDevolverFalse</t>
-  </si>
-  <si>
     <t>La Geolocalización se encuentra a más de 5 cuadras de la sucursal del banco</t>
   </si>
   <si>
-    <t>SucursalBanco - dadaUnaGeolocalizacionDentroDelRangoEsCercanoDebeDevolverTrue</t>
-  </si>
-  <si>
     <t>La Geolocalización se encuentra a menos de 5 cuadras de la sucursal del banco</t>
   </si>
   <si>
     <t>Consultar por disponibilidad</t>
   </si>
   <si>
-    <t>LocalComercial - siendoUnaFechaFueraDelHorarioDeAtencionDeUnLocalNoDebeEstarDisponible</t>
-  </si>
-  <si>
     <t>La fecha y hora de consulta no está contenida en el horario de atención</t>
   </si>
   <si>
     <t>El POI no debe estar disponible</t>
   </si>
   <si>
-    <t>LocalComercial - siendoUnaFechadentroDelHorarioDeAtencionDeUnLocalDebeEstarDisponible</t>
-  </si>
-  <si>
     <t>La fecha y hora de consulta está contenida en el horario de atención</t>
   </si>
   <si>
     <t>El POI debe estar disponible</t>
   </si>
   <si>
-    <t>PENDIENTES</t>
-  </si>
-  <si>
     <t>Buscar Puntos de Interés</t>
   </si>
   <si>
-    <t>CGP - dadaUnaPalabraCoincidenteConUnServicioTienePalabraDebeDevolverTrue</t>
-  </si>
-  <si>
     <t>La palabra coincide con un servicio</t>
   </si>
   <si>
     <t>El POI debe tener la palabra</t>
   </si>
   <si>
-    <t>CGP - dadaUnaPalabraIncluidaEnPalabrasClaveTienePalabraDebeDevolverTrue</t>
-  </si>
-  <si>
     <t>La palabra es una de las palabras claves</t>
   </si>
   <si>
-    <t>CGP - dadaUnaPalabraCualquieraTienePalabraDebeDevolverFalse</t>
-  </si>
-  <si>
     <t>La palabra no pertenece ni a los servicios, ni a las palabras clave</t>
   </si>
   <si>
     <t>El POI no debe tener la palabra</t>
   </si>
   <si>
-    <t>LocalComercial - dadaUnaPalabraLibreriaEscolarTienePalabraDebeCoincidirConNombre</t>
-  </si>
-  <si>
     <t>La palabra coincide con el nombre</t>
   </si>
   <si>
-    <t>LocalComercial - dadaUnaPalabraContenidaEnElNombreDelRubroLibreriaEscolarDebeTenerLaPalabra</t>
-  </si>
-  <si>
     <t>La palabra coincide con el rubro</t>
   </si>
   <si>
-    <t>LocalComercial - dadaUnaPalabraQueNoEsClaveNiDelRubroNiDelNombreLibreriaEscolarNoDebeTenerEsaPalabra</t>
-  </si>
-  <si>
     <t>La palabra no coincide ni con el nombre ni con el rubro</t>
   </si>
   <si>
-    <t>ParadaColectivo - dadaUnaPalabraIgualASuLineaTienePalabraDebeDevolverTrue</t>
-  </si>
-  <si>
     <t>La palabra coincide con la línea</t>
   </si>
   <si>
-    <t>ParadaColectivo - dadaUnaPalabraClaveExistenteTienePalabraDebeDevolverTrue</t>
-  </si>
-  <si>
     <t>La palabra coincide con una palabra clave</t>
   </si>
   <si>
-    <t>ParadaColectivo - dadaUnaPalabraCualquieraNoIncluidaEnNingunConjuntoTienePalabraDebeDevolverFalse</t>
-  </si>
-  <si>
     <t>La palabra no coincide ni con la línea, ni con las palabras clave</t>
   </si>
   <si>
-    <t>SucursalBanco - dadaUnaPalabraCoincidenteConElBancoTienePalabraDebeDevolverTrue</t>
-  </si>
-  <si>
     <t>la palabra coincide con el nombre del banco</t>
   </si>
   <si>
-    <t>SucursalBanco - dadaUnaPalabraCoincidenteConUnServicioTienePalabraDebeDevolverTrue</t>
-  </si>
-  <si>
     <t>la palabra coincide con un servicio</t>
   </si>
   <si>
-    <t>SucursalBanco - dadaUnaPalabraIncluidaEnPalabrasClaveTienePalabraDebeDevolverTrue</t>
-  </si>
-  <si>
     <t>la palabra coincide con una palabra clave</t>
   </si>
   <si>
-    <t>SucursalBanco - dadaUnaPalabraCualquieraTienePalabraDebeDevolverFalse</t>
-  </si>
-  <si>
     <t>la palabra no coincide ni con el nombre del banco, ni con un servicio, ni con las palabras claves</t>
   </si>
   <si>
-    <t>TerminalInteractiva - BuscarYEncontrarPOIKiosco</t>
-  </si>
-  <si>
     <t>el POI se encuentra en la la colección de puntos de interés de la Terminal y la palabra de búsqueda coincide con el Rubro del POI</t>
   </si>
   <si>
     <t>La búsqueda tiene que tener 1 resultado, y este debe ser el Local</t>
   </si>
   <si>
-    <t>TerminalInteractiva - BuscarYEncontrarPOIKioscoPorPalabraClave</t>
-  </si>
-  <si>
     <t>el POI se encuentra en la la colección de puntos de interés de la Terminal y la palabra de búsqueda con una palabra clave del POI</t>
   </si>
   <si>
-    <t>TerminalInteractiva - BuscarYNoEncontrarNingunPOI</t>
-  </si>
-  <si>
-    <t>el POI se encuentra en la la colección de puntos de interés de la Terminal y el POI no tiene la palabra de búsqueda</t>
-  </si>
-  <si>
     <t>La búsqueda no tiene que arrojar resultados</t>
   </si>
   <si>
@@ -235,13 +151,118 @@
   </si>
   <si>
     <t>El POI debe responder que no es cercano</t>
+  </si>
+  <si>
+    <t>CGP - Preguntar si esCercano con una Geolocalizacion dentro del rango</t>
+  </si>
+  <si>
+    <t>LocalComercial - Preguntar si esCercano con una Geolocalizacion dentro del rango</t>
+  </si>
+  <si>
+    <t>ParadaColectivo - Preguntar si esCercano con una Geolocalizacion dentro del rango</t>
+  </si>
+  <si>
+    <t>SucursalBanco - Preguntar si esCercano con una Geolocalizacion dentro del rango</t>
+  </si>
+  <si>
+    <t>LocalComercial - Preguntar si esCercano con una Geolocalización fuera del rango</t>
+  </si>
+  <si>
+    <t>ParadaColectivo - Preguntar si esCercano con una Geolocalización fuera del rango</t>
+  </si>
+  <si>
+    <t>SucursalBanco - Preguntar si esCercano con una Geolocalización fuera del rango</t>
+  </si>
+  <si>
+    <t>La Geolocalización no pertenece a la comuna del CGP</t>
+  </si>
+  <si>
+    <t>CGP - Preguntar si tienePalabra con una palabra que coincide con una palabra clave</t>
+  </si>
+  <si>
+    <t>LocalComercial - Preguntar si tienePalabra con una palabra que coincide con el nombre</t>
+  </si>
+  <si>
+    <t>LocalComercial - Preguntar si tienePalabra con una palabra que coincide con el rubro</t>
+  </si>
+  <si>
+    <t>CGP - Preguntar si tienePalabra con una palabra cualquiera</t>
+  </si>
+  <si>
+    <t>LocalComercial - Preguntar si tienePalabra con una palabra  cualquiera</t>
+  </si>
+  <si>
+    <t>Parada Colectivo - Preguntar si tienePalabra con una palabra que coincide con la linea</t>
+  </si>
+  <si>
+    <t>ParadaColectivo - Preguntar si tienePalabra con una palabra  cualquiera</t>
+  </si>
+  <si>
+    <t>Parada Colectivo - Preguntar si tienePalabra con una palabra que coincide con una palabra clave</t>
+  </si>
+  <si>
+    <t>SucursalBanco - Preguntar si tienePalabra con una palabra  cualquiera</t>
+  </si>
+  <si>
+    <t>SucursalBanco - Preguntar si tienePalabra con una palabra que coincide con el banco</t>
+  </si>
+  <si>
+    <t>SucursalBanco - Preguntar si tienePalabra con una palabra que coincide con un servicio</t>
+  </si>
+  <si>
+    <t>CGP - Preguntar si tienePalabra con una palabra que coincide con un servicio</t>
+  </si>
+  <si>
+    <t>SucursalBanco - Preguntar si tienePalabra con una palabra que coincide con una palabra clave</t>
+  </si>
+  <si>
+    <t>TerminalInteractiva - Encontrar POI a traves de la busqueda segun una palabra del POI</t>
+  </si>
+  <si>
+    <t>TerminalInteractiva - Encontrar POI a traves de la busqueda segun un rubro del POI</t>
+  </si>
+  <si>
+    <t>TerminalInteractiva - No encontrar ningún POI a través de una búsqueda con una palabra cualquiera</t>
+  </si>
+  <si>
+    <t>el POI se encuentra en la colección de puntos de interés de la Terminal y el POI no tiene la palabra de búsqueda</t>
+  </si>
+  <si>
+    <t>LocalComercial - Preguntar si estaDisponible con una fecha dentro del horario de atención</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocalComercial - Preguntar si estaDisponible con una fecha fuera del horario de atención </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CGP - Preguntar si estaDisponible con una fecha fuera del horario de atención </t>
+  </si>
+  <si>
+    <t>CGP - Preguntar si estaDisponible con una fecha dentro del horario de atención de un servicio</t>
+  </si>
+  <si>
+    <t>SucursalBancaria - Preguntar si estaDisponible con una fecha dentro del horario bancario</t>
+  </si>
+  <si>
+    <t>SucursalBancaria - Preguntar si estaDisponible con una fecha dentro del horario de un servicio</t>
+  </si>
+  <si>
+    <t>SucursalBancaria - Preguntar si estaDisponible con una fecha fuera del horario de anteción</t>
+  </si>
+  <si>
+    <t>La fecha y hora de consulta está contenida en el horario de atención de un servicio</t>
+  </si>
+  <si>
+    <t>La fecha y hora de consulta no está contenida en el horario de atención de la sucursal ni de sus servicio</t>
+  </si>
+  <si>
+    <t>La fecha y hora de consulta está contenida en el horario de atención de la sucursal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -255,6 +276,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -335,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -357,6 +383,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,18 +669,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="33.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" customWidth="1"/>
+    <col min="4" max="4" width="56.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -659,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -679,463 +713,561 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3"/>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3"/>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3"/>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3"/>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3"/>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3"/>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
-      <c r="B11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="3"/>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
-      <c r="B13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="B14" s="3">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="9">
+        <v>14</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>8</v>
+      <c r="A16" s="8"/>
+      <c r="B16" s="10">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="3"/>
+      <c r="A17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
-      <c r="B18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="3"/>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
-      <c r="B19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="3"/>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
-      <c r="B20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="3"/>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="D20" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
-      <c r="B21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="3"/>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
-      <c r="B22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="3"/>
+      <c r="B22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
-      <c r="B23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="3"/>
+      <c r="B23" s="2">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="D23" s="2" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
-      <c r="B24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="3"/>
+      <c r="B24" s="2">
+        <v>23</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="D24" s="2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
-      <c r="B25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="3"/>
+      <c r="B25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="D25" s="2" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
-      <c r="B26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="3"/>
+      <c r="B26" s="2">
+        <v>25</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="D26" s="2" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
-      <c r="B27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="3"/>
+      <c r="B27" s="2">
+        <v>26</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="D27" s="2" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
-      <c r="B28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="3"/>
+      <c r="B28" s="2">
+        <v>27</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="D28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="7"/>
+      <c r="B29" s="2">
+        <v>28</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="3"/>
       <c r="D29" s="2" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
-      <c r="B30" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="3"/>
+      <c r="B30" s="2">
+        <v>29</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+      <c r="B31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="3"/>
       <c r="D31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="2">
+        <v>31</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="E32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
@@ -1161,13 +1293,21 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A16:A31"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A17:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>